<commit_message>
Fix tables with two rank columns
</commit_message>
<xml_diff>
--- a/src/data/facts-and-figures.xlsx
+++ b/src/data/facts-and-figures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ColbyPastre\Local Sites\tax-foundation-development-site\app\public\wp-content\themes\facts-and-figures-web\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB51C11-77E3-4382-A433-8C9D15D76316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085B84DE-03F6-41E8-BA95-322DA5B3E529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="18" activeTab="22" xr2:uid="{E1FAFE64-C91F-4801-9C00-8657359E225A}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3076" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3076" uniqueCount="711">
   <si>
     <t>Table 1.</t>
   </si>
@@ -2329,7 +2329,19 @@
     <t>(f) Nebraska's corporation occupation tax is due every other year. The maximum tax is $23,990 for domestic (Nebraska) corporations and $30,000 for foreign (out-of-state) corporations.</t>
   </si>
   <si>
-    <t>Note: Excise taxes are special taxes on specific goods or activities—such as gasoline, tobacco, or gambling—rather than general tax bases such as income or consumption. Excise taxes are often included in the final price of products and services, and are hidden to consumers. In order to determine the the average tax rate on a gallon of fuel, rates may include any of the following: excise taxes, environmental fees, storage tank taxes, other fees or taxes, and general sales tax. In states where gasoline is subject to the general sales tax, or where the fuel tax is based on the average sale price, the average rate is sensitive to changes in the price of gasoline. States that fully or partially apply general sales taxes to gasoline are California, Connecticut, Illinois, Indiana, Michigan, and New York. D.C.’s rank does not affect states’ ranks, but the figure in parentheses indicates where it would rank if included.</t>
+    <t>State Rank</t>
+  </si>
+  <si>
+    <t>Combined Rank</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gas Tax Rank</t>
+  </si>
+  <si>
+    <t>Total Rank</t>
+  </si>
+  <si>
+    <t>Note: Excise taxes are special taxes on specific goods or activities—such as gasoline, tobacco, or gambling—rather than general tax bases such as income or consumption. Excise taxes are often included in the final price of products and services, and are hidden to consumers. In order to determine the average tax rate on a gallon of fuel, rates may include any of the following: excise taxes, environmental fees, storage tank taxes, other fees or taxes, and general sales tax. In states where gasoline is subject to the general sales tax, or where the fuel tax is based on the average sale price, the average rate is sensitive to changes in the price of gasoline. States that fully or partially apply general sales taxes to gasoline are California, Connecticut, Illinois, Indiana, Michigan, and New York. D.C.’s rank does not affect states’ ranks, but the figure in parentheses indicates where it would rank if included.</t>
   </si>
 </sst>
 </file>
@@ -31506,9 +31518,9 @@
   <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F17" sqref="F17"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31565,7 +31577,7 @@
         <v>279</v>
       </c>
       <c r="C5" s="223" t="s">
-        <v>5</v>
+        <v>706</v>
       </c>
       <c r="D5" s="223" t="s">
         <v>280</v>
@@ -31574,7 +31586,7 @@
         <v>281</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>5</v>
+        <v>707</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="199"/>
@@ -36582,7 +36594,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -37576,7 +37588,7 @@
     </row>
     <row r="62" spans="1:11" ht="159.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="463" t="s">
-        <v>706</v>
+        <v>710</v>
       </c>
       <c r="B62" s="463"/>
       <c r="C62" s="463"/>
@@ -37609,8 +37621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD00CA32-C333-45F9-9935-4504CB2E91D4}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -37673,7 +37685,7 @@
         <v>338</v>
       </c>
       <c r="C6" s="411" t="s">
-        <v>5</v>
+        <v>708</v>
       </c>
       <c r="D6" s="411" t="s">
         <v>339</v>
@@ -37682,7 +37694,7 @@
         <v>340</v>
       </c>
       <c r="F6" s="411" t="s">
-        <v>5</v>
+        <v>709</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix Table 3 - SBTCI
Data fix. Also updates to minor new version of npm.
</commit_message>
<xml_diff>
--- a/src/data/facts-and-figures.xlsx
+++ b/src/data/facts-and-figures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\wp-content\themes\facts-and-figures-web\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ColbyPastre\Local Sites\tax-foundation-development-site\app\public\wp-content\themes\facts-and-figures-web\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C46A8FF-68EE-4894-82D9-3922BEB77444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EB0C3C-F32D-4F56-A64D-1EA7527E1277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7650" yWindow="2760" windowWidth="18930" windowHeight="15690" firstSheet="28" activeTab="42" xr2:uid="{E1FAFE64-C91F-4801-9C00-8657359E225A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="3" activeTab="3" xr2:uid="{E1FAFE64-C91F-4801-9C00-8657359E225A}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="44" r:id="rId1"/>
@@ -4400,9 +4400,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4440,7 +4440,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4546,7 +4546,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4688,7 +4688,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -41105,17 +41105,17 @@
     <row r="83" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A67:D71"/>
     <mergeCell ref="A61:D61"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A67:D71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" orientation="portrait" r:id="rId1"/>
@@ -49620,10 +49620,10 @@
   </sheetPr>
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F36" sqref="F36"/>
-      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -49721,7 +49721,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="11">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="11">
         <v>19</v>
@@ -49759,7 +49759,7 @@
         <v>48</v>
       </c>
       <c r="H8" s="14">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="14.25" x14ac:dyDescent="0.2">
@@ -49791,7 +49791,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="14">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="14">
         <v>28</v>
@@ -49864,7 +49864,7 @@
         <v>47</v>
       </c>
       <c r="D13" s="11">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="11">
         <v>46</v>
@@ -49884,7 +49884,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="14">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D14" s="14">
         <v>50</v>
@@ -49945,7 +49945,7 @@
         <v>34</v>
       </c>
       <c r="H16" s="14">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -49968,7 +49968,7 @@
         <v>41</v>
       </c>
       <c r="H17" s="11">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -49999,7 +49999,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="11">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="11">
         <v>43</v>
@@ -50051,7 +50051,7 @@
         <v>29</v>
       </c>
       <c r="E21" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F21" s="11">
         <v>15</v>
@@ -50074,7 +50074,7 @@
         <v>21</v>
       </c>
       <c r="E22" s="14">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F22" s="14">
         <v>29</v>
@@ -50114,13 +50114,13 @@
         <v>24</v>
       </c>
       <c r="C24" s="14">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D24" s="14">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E24" s="14">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F24" s="14">
         <v>48</v>
@@ -50143,7 +50143,7 @@
         <v>35</v>
       </c>
       <c r="E25" s="11">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F25" s="11">
         <v>8</v>
@@ -50163,7 +50163,7 @@
         <v>45</v>
       </c>
       <c r="D26" s="14">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="14">
         <v>45</v>
@@ -50206,7 +50206,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D28" s="14">
         <v>20</v>
@@ -50221,7 +50221,7 @@
         <v>7</v>
       </c>
       <c r="H28" s="14">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -50252,13 +50252,13 @@
         <v>30</v>
       </c>
       <c r="C30" s="14">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D30" s="14">
         <v>8</v>
       </c>
       <c r="E30" s="14">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F30" s="14">
         <v>25</v>
@@ -50275,13 +50275,13 @@
         <v>31</v>
       </c>
       <c r="C31" s="11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31" s="11">
         <v>3</v>
       </c>
       <c r="E31" s="11">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F31" s="11">
         <v>30</v>
@@ -50321,10 +50321,10 @@
         <v>33</v>
       </c>
       <c r="C33" s="11">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D33" s="11">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E33" s="11">
         <v>32</v>
@@ -50413,7 +50413,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="11">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D37" s="11">
         <v>13</v>
@@ -50488,7 +50488,7 @@
         <v>10</v>
       </c>
       <c r="E40" s="14">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F40" s="14">
         <v>32</v>
@@ -50534,7 +50534,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="14">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F42" s="14">
         <v>38</v>
@@ -50574,13 +50574,13 @@
         <v>44</v>
       </c>
       <c r="C44" s="14">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D44" s="14">
         <v>41</v>
       </c>
       <c r="E44" s="14">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F44" s="14">
         <v>16</v>
@@ -50626,7 +50626,7 @@
         <v>6</v>
       </c>
       <c r="E46" s="14">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F46" s="14">
         <v>33</v>
@@ -50658,7 +50658,7 @@
         <v>35</v>
       </c>
       <c r="H47" s="11">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -50773,7 +50773,7 @@
         <v>36</v>
       </c>
       <c r="H52" s="14">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -50804,13 +50804,13 @@
         <v>54</v>
       </c>
       <c r="C54" s="14">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D54" s="14">
         <v>17</v>
       </c>
       <c r="E54" s="14">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F54" s="14">
         <v>24</v>
@@ -50830,7 +50830,7 @@
         <v>24</v>
       </c>
       <c r="D55" s="11">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E55" s="11">
         <v>38</v>
@@ -53297,7 +53297,7 @@
   </sheetPr>
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>

</xml_diff>